<commit_message>
1. Updated Element Locators 2. Added GoogleHelper for book search 3. Added JS helper
</commit_message>
<xml_diff>
--- a/goodreads/src/main/resources/Sanity.xlsx
+++ b/goodreads/src/main/resources/Sanity.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\Desktop\TV\Automation_Project\goodreads\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\Desktop\TestVagrant\2\Automation_Project\goodreads\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F2754E-5C33-4C9A-853A-52331BFED221}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD7DB743-02B4-42AD-B771-FB9EBE9C968C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,10 +66,10 @@
     <t>com.testvagrant.goodreads.WhatsTheBookName</t>
   </si>
   <si>
-    <t>Sample.xlsx</t>
-  </si>
-  <si>
     <t>TestCaseMaster</t>
+  </si>
+  <si>
+    <t>tweet.xlsx</t>
   </si>
 </sst>
 </file>
@@ -483,10 +483,10 @@
         <v>11</v>
       </c>
       <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
         <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>7</v>

</xml_diff>